<commit_message>
Optimize the method LaunchApplication and CloseApplication
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST2801_AlarmUnderMaintenanceMode.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST2801_AlarmUnderMaintenanceMode.xlsx
@@ -4053,10 +4053,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$SNMP_GXT_0_NAME$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$SNMP_GXT_Ip_Port$</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4086,6 +4082,10 @@
   </si>
   <si>
     <t>$SNMP_SinAuto_0$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$SNMP_device_0_NAME$</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4637,8 +4637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B175" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H107" sqref="H107"/>
+    <sheetView tabSelected="1" topLeftCell="B125" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I150" sqref="I150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4879,10 +4879,10 @@
         <v>856</v>
       </c>
       <c r="I8" s="4" t="s">
+        <v>910</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>911</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>912</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>857</v>
@@ -5504,7 +5504,7 @@
         <v>4</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -5821,7 +5821,7 @@
         <v>2</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
@@ -6174,13 +6174,13 @@
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
       <c r="H59" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I59" s="9">
         <v>1</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
@@ -6459,15 +6459,15 @@
         <v>861</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="F71" s="4"/>
       <c r="G71" s="9"/>
       <c r="H71" s="4" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="J71" s="4" t="b">
         <v>1</v>
@@ -6560,7 +6560,7 @@
         <v>56</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
@@ -6858,13 +6858,13 @@
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I88" s="9">
         <v>1</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
@@ -7108,7 +7108,7 @@
         <v>871</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
@@ -7244,7 +7244,7 @@
         <v>56</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I104" s="4"/>
       <c r="J104" s="4"/>
@@ -7542,13 +7542,13 @@
       <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I117" s="9">
         <v>1</v>
       </c>
       <c r="J117" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="K117" s="4"/>
       <c r="L117" s="4"/>
@@ -7792,7 +7792,7 @@
         <v>897</v>
       </c>
       <c r="J127" s="4" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="K127" s="4"/>
       <c r="L127" s="4"/>
@@ -8034,13 +8034,13 @@
       <c r="F138" s="4"/>
       <c r="G138" s="4"/>
       <c r="H138" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I138" s="9">
         <v>1</v>
       </c>
       <c r="J138" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="K138" s="4"/>
       <c r="L138" s="4"/>
@@ -8327,7 +8327,7 @@
         <v>887</v>
       </c>
       <c r="I150" s="4" t="s">
-        <v>904</v>
+        <v>912</v>
       </c>
       <c r="J150" s="4" t="b">
         <v>1</v>
@@ -8420,7 +8420,7 @@
         <v>56</v>
       </c>
       <c r="H154" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I154" s="4"/>
       <c r="J154" s="4"/>
@@ -8718,13 +8718,13 @@
       <c r="F167" s="4"/>
       <c r="G167" s="4"/>
       <c r="H167" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I167" s="9">
         <v>1</v>
       </c>
       <c r="J167" s="4" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="K167" s="4"/>
       <c r="L167" s="4"/>
@@ -8968,7 +8968,7 @@
         <v>871</v>
       </c>
       <c r="J177" s="4" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="K177" s="4"/>
       <c r="L177" s="4"/>
@@ -9104,7 +9104,7 @@
         <v>56</v>
       </c>
       <c r="H183" s="4" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="I183" s="4"/>
       <c r="J183" s="4"/>
@@ -9402,13 +9402,13 @@
       <c r="F196" s="4"/>
       <c r="G196" s="4"/>
       <c r="H196" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="I196" s="9">
         <v>1</v>
       </c>
       <c r="J196" s="4" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="K196" s="4"/>
       <c r="L196" s="4"/>
@@ -9652,7 +9652,7 @@
         <v>897</v>
       </c>
       <c r="J206" s="4" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="K206" s="4"/>
       <c r="L206" s="4"/>

</xml_diff>